<commit_message>
add script for audio replacement
</commit_message>
<xml_diff>
--- a/survey/PhenomX Health Women's Survey (All Responses).xlsx
+++ b/survey/PhenomX Health Women's Survey (All Responses).xlsx
@@ -13,8 +13,28 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="C45">
+      <text>
+        <t xml:space="preserve">Responder updated this value.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="AH45">
+      <text>
+        <t xml:space="preserve">Responder updated this value.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="505">
   <si>
     <t>Timestamp</t>
   </si>
@@ -631,6 +651,270 @@
     <t>michelc@drit.ml</t>
   </si>
   <si>
+    <t>Bloating, Gas, Mood swings, Headaches, Low energy, fatigue, Weight gain, Incontinence, Skin wrinkling, Dry skin, Dry mouth, Decreased memory, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t>I am aware of general healthy ways and try to stick to them, I consulted a nutritionist and have a personalized plan to follow</t>
+  </si>
+  <si>
+    <t>marzia.massignani@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland </t>
+  </si>
+  <si>
+    <t>Quality of advice not sufficient</t>
+  </si>
+  <si>
+    <t>Time spent</t>
+  </si>
+  <si>
+    <t>Bloating, Constipation, Mood swings, Anxiety and/or panic attacks, Sleep difficulties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I ask for advice when in the pharmacy, I have a nutritionist friend. </t>
+  </si>
+  <si>
+    <t>Fast results addressing current issues, Preventive plan, Focus on optimal weight</t>
+  </si>
+  <si>
+    <t>Cotrutadiana@yahoo.com</t>
+  </si>
+  <si>
+    <t>Quality of advice not sufficient, Time spent</t>
+  </si>
+  <si>
+    <t>Quality of advice not sufficient, Money spent</t>
+  </si>
+  <si>
+    <t>Menstrual cramps, Depression, Brain fog, Anxiety and/or panic attacks, Sleep difficulties, Low energy, fatigue, skin rash and atopic dermatitis</t>
+  </si>
+  <si>
+    <t>based on biological dosage only</t>
+  </si>
+  <si>
+    <t>it should be certified and prove its efficiency through a trial like a clinical trial</t>
+  </si>
+  <si>
+    <t>algorithm that send me a weekly summary through the channel and the day I choose.</t>
+  </si>
+  <si>
+    <t>regarding the microbiome assessment, there is no international standard so far, I am a microbiologist :-) There is an overuse of this word now a buzz word.</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Gas, Menstrual cramps, Night sweats, Low energy, fatigue, Vaginal dryness</t>
+  </si>
+  <si>
+    <t>Focus on optimal weight, Advice on healthy recipes</t>
+  </si>
+  <si>
+    <t>Pascalehellmueller66@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suisse 🇨🇭 </t>
+  </si>
+  <si>
+    <t>Brain fog, Sleep difficulties, Low energy, fatigue, Weight gain, Decreased memory</t>
+  </si>
+  <si>
+    <t>Personalized recommendations without going to any specialists, One- click purchase of food supplements of trusted brands</t>
+  </si>
+  <si>
+    <t>caroline.munari@me.com</t>
+  </si>
+  <si>
+    <t>Sore breasts, Gas, Constipation, Weight gain, Age spots, melasma</t>
+  </si>
+  <si>
+    <t>Connection with people who are at the same stage in their lives or have just been through it, Personalized recommendations without going to any specialists</t>
+  </si>
+  <si>
+    <t>Clear everyday plan easy to follow, Focus on optimal weight</t>
+  </si>
+  <si>
+    <t>Sore breasts, Menstrual cramps, Low energy, fatigue, Weight gain, Skin wrinkling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General recommendations on how to address symptoms of menopause with the help of nutrition, Personalized recommendations without going to any specialists, One- click purchase of food supplements of trusted brands, Follow progress of symptoms overtime and get charts to see if any improvment, could be could to include an index which gives you the state  of your profile compared to the level you should be  </t>
+  </si>
+  <si>
+    <t>It saves time, It is private, You can have holistic approach instead of going to each specialist</t>
+  </si>
+  <si>
+    <t>celine.dicara@wanadoo.fr</t>
+  </si>
+  <si>
+    <t>Mood swings, Sleep difficulties, Low energy, fatigue, Weight gain</t>
+  </si>
+  <si>
+    <t>Clear everyday plan easy to follow, Preventive plan, Focus on optimal weight, Advice on healthy recipes</t>
+  </si>
+  <si>
+    <t>maura.boucher@comcast.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are so welcome! </t>
+  </si>
+  <si>
+    <t>Night sweats, Headaches, Anxiety and/or panic attacks, Sleep difficulties, Low energy, fatigue</t>
+  </si>
+  <si>
+    <t>I am aware of general healthy ways and try to stick to them, I consulted a nutritionist and have a personalized plan to follow, I follow advice from my doctors</t>
+  </si>
+  <si>
+    <t>Personalized recommendations without going to any specialists, Network of certified trusted nutritionists for online consultation, One- click purchase of food supplements of trusted brands</t>
+  </si>
+  <si>
+    <t>It saves time, It is private, i can choose when to do it / works with my schedule</t>
+  </si>
+  <si>
+    <t>esvanas@gmail.com</t>
+  </si>
+  <si>
+    <t>Convenience of service</t>
+  </si>
+  <si>
+    <t>Quality of advice not sufficient, Convenience of service, Money spent</t>
+  </si>
+  <si>
+    <t>Bloating, Gas, Constipation, Night sweats, Body odor, Mood swings, Headaches, Sleep difficulties, Joint pain, Low energy, fatigue, Weight gain, Loss of skin elasticity, sagging skin, Skin wrinkling, Dry skin</t>
+  </si>
+  <si>
+    <t>I am aware of general healthy ways and try to stick to them, I consulted a nutritionist and have a personalized plan to follow, Acupuncture</t>
+  </si>
+  <si>
+    <t>General recommendations on how to address symptoms of menopause with the help of nutrition, Connection with people who are at the same stage in their lives or have just been through it, Personalized recommendations without going to any specialists, Network of certified trusted nutritionists for online consultation, One- click purchase of food supplements of trusted brands</t>
+  </si>
+  <si>
+    <t>nutritionist</t>
+  </si>
+  <si>
+    <t>It saves time, Easy &amp; convenient</t>
+  </si>
+  <si>
+    <t>Clear everyday plan easy to follow, Fast results addressing current issues, Focus on optimal weight, Advice on healthy recipes</t>
+  </si>
+  <si>
+    <t>lisahgable@gmail.com</t>
+  </si>
+  <si>
+    <t>Thank you! As someone who had a hysterectomy at age 37, I have done a lot of research and tried many different treatments. Feel free to reach out with any questions as I fully support this app!</t>
+  </si>
+  <si>
+    <t>Constipation, Headaches, Low energy, fatigue, Loss of skin elasticity, sagging skin, Skin wrinkling</t>
+  </si>
+  <si>
+    <t>paulajanenenn@yahoo.com</t>
+  </si>
+  <si>
+    <t>Most welcome. I spend little on healthcare because it’s free in the UK</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Dry skin</t>
+  </si>
+  <si>
+    <t>Preventive plan, Advice on healthy recipes</t>
+  </si>
+  <si>
+    <t>Andreea.sincu@gmail.com</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Bloating, Gas</t>
+  </si>
+  <si>
+    <t>laura_mantu@yahoo.com</t>
+  </si>
+  <si>
+    <t>You re welcome</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Mood swings, Joint pain, Age spots, melasma, Dry skin, Vaginal dryness</t>
+  </si>
+  <si>
+    <t>masha_verhoogt@yahoo.com</t>
+  </si>
+  <si>
+    <t>Thank you🙏🙂</t>
+  </si>
+  <si>
+    <t>Bloating, Gas, Night sweats, Body odor, Mood swings, Brain fog, Sleep difficulties, Joint pain, Low energy, fatigue, Frequent sickness - colds, flu, etc., Loss of skin elasticity, sagging skin, Age spots, melasma, Dry skin, Decreased memory</t>
+  </si>
+  <si>
+    <t>ioanac.cofaru@gmail.com</t>
+  </si>
+  <si>
+    <t>Thank you too!</t>
+  </si>
+  <si>
+    <t>The Netherlands</t>
+  </si>
+  <si>
+    <t>Bloating</t>
+  </si>
+  <si>
+    <t>I only listen to my body and follow its needs, I am aware of general healthy ways and try to stick to them, I follow advice from my doctors</t>
+  </si>
+  <si>
+    <t>monicamilosescu@gmail.com</t>
+  </si>
+  <si>
+    <t>You are welcomr!</t>
+  </si>
+  <si>
+    <t>Sleep difficulties, Low energy, fatigue, Loss of skin elasticity, sagging skin, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t>General recommendations on how to address symptoms of menopause with the help of nutrition, Connection with people who are at the same stage in their lives or have just been through it, Personalized recommendations without going to any specialists, One- click purchase of food supplements of trusted brands</t>
+  </si>
+  <si>
+    <t>dara.sosulski@gmail.com</t>
+  </si>
+  <si>
+    <t>You're very welcome!</t>
+  </si>
+  <si>
+    <t>Headaches, Weight gain, Loss of skin elasticity, sagging skin, Skin wrinkling, Age spots, melasma, Vaginal dryness, Decreased memory</t>
+  </si>
+  <si>
+    <t>telford515@yahoo.com</t>
+  </si>
+  <si>
+    <t>None of the above</t>
+  </si>
+  <si>
+    <t>Gas, Vaginal dryness</t>
+  </si>
+  <si>
+    <t>I follow advice from my doctors</t>
+  </si>
+  <si>
+    <t>Preventive plan, Focus on optimal weight</t>
+  </si>
+  <si>
+    <t>Sleep difficulties, Skin wrinkling, Vaginal dryness</t>
+  </si>
+  <si>
+    <t>General recommendations on how to address symptoms of menopause with the help of nutrition, Connection with people who are at the same stage in their lives or have just been through it</t>
+  </si>
+  <si>
+    <t>patrbegley@gmail.com</t>
+  </si>
+  <si>
+    <t>Thank you for inquiring</t>
+  </si>
+  <si>
     <t>8a. Do you enjoy its look and feel?</t>
   </si>
   <si>
@@ -760,18 +1044,9 @@
     <t>Gas, Constipation, Brain fog, Hair loss, thinning, change in texture</t>
   </si>
   <si>
-    <t>Personalized recommendations without going to any specialists, One- click purchase of food supplements of trusted brands</t>
-  </si>
-  <si>
-    <t>Bloating</t>
-  </si>
-  <si>
     <t>I only listen to my body and follow its needs, I follow advice from my doctors</t>
   </si>
   <si>
-    <t>None of the above</t>
-  </si>
-  <si>
     <t>I am aware of general healthy ways and try to stick to them, I use labs to also inform my decisions</t>
   </si>
   <si>
@@ -796,9 +1071,6 @@
     <t xml:space="preserve">It saves time, Less expensive </t>
   </si>
   <si>
-    <t>Clear everyday plan easy to follow, Focus on optimal weight</t>
-  </si>
-  <si>
     <t>Menstrual cramps, Headaches, Low energy, fatigue, Dry skin, Dry mouth</t>
   </si>
   <si>
@@ -820,9 +1092,6 @@
     <t>I only listen to my body and follow its needs, I am aware of general healthy ways and try to stick to them, I ask for advice when in the pharmacy</t>
   </si>
   <si>
-    <t>General recommendations on how to address symptoms of menopause with the help of nutrition, Connection with people who are at the same stage in their lives or have just been through it, Personalized recommendations without going to any specialists, One- click purchase of food supplements of trusted brands</t>
-  </si>
-  <si>
     <t>Joint pain, Low energy, fatigue, Weight gain, Skin wrinkling</t>
   </si>
   <si>
@@ -847,9 +1116,6 @@
     <t>I would need to see it more in detail and try out the functionalities and the general feel of it.</t>
   </si>
   <si>
-    <t>Fast results addressing current issues, Preventive plan, Focus on optimal weight</t>
-  </si>
-  <si>
     <t>lskavska@hotmail.com</t>
   </si>
   <si>
@@ -925,9 +1191,6 @@
     <t xml:space="preserve">It saves time, Drs rdvs are a pain to make </t>
   </si>
   <si>
-    <t>Clear everyday plan easy to follow, Fast results addressing current issues, Focus on optimal weight, Advice on healthy recipes</t>
-  </si>
-  <si>
     <t>megandaypb@gmail.com</t>
   </si>
   <si>
@@ -941,9 +1204,6 @@
   </si>
   <si>
     <t>Night sweats, Hot flashes, Brain fog, Low energy, fatigue, Weight gain</t>
-  </si>
-  <si>
-    <t>I only listen to my body and follow its needs, I am aware of general healthy ways and try to stick to them, I follow advice from my doctors</t>
   </si>
   <si>
     <t>Menstrual cramps, Depression, Anxiety and/or panic attacks, Low energy, fatigue, Skin wrinkling, Age spots, melasma, Vaginal dryness, Decreased memory</t>
@@ -968,9 +1228,6 @@
     <t>Sleep difficulties, Weight gain, Allergy</t>
   </si>
   <si>
-    <t>Clear everyday plan easy to follow, Preventive plan, Focus on optimal weight, Advice on healthy recipes</t>
-  </si>
-  <si>
     <t>Germidal@gmail.com</t>
   </si>
   <si>
@@ -998,9 +1255,6 @@
     <t xml:space="preserve">Don't like the beige background.  I use the lifesum app and like the look and feel.   </t>
   </si>
   <si>
-    <t xml:space="preserve">Switzerland </t>
-  </si>
-  <si>
     <t>Bloating, Gas, Constipation, Mood swings, Sleep difficulties, Low energy, fatigue, Weight gain, Skin wrinkling</t>
   </si>
   <si>
@@ -1133,12 +1387,6 @@
     <t>You are welcome, such an app could be a great preventive tool for women who believe they are not yet even in pre menopause, while this stage can come more quickly than thought, and entails symptoms that usually are not even diagnosed well by GPs (they make unnecessary neuro tests when headaches come, or believe there is a problem of stress), if the app could in some ways with functionalities other than official menopause such as nutritional /healthy recommendations for various ages, that helps onboarding earlier the women users 40-70</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Quality of advice not sufficient</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -1148,16 +1396,163 @@
     <t>I would probably work on the My Recommendations page a bit more and its colors.</t>
   </si>
   <si>
-    <t>Preventive plan, Focus on optimal weight</t>
-  </si>
-  <si>
     <t>szilvike.varga@gmail.com</t>
   </si>
   <si>
     <t>Thank you for your effort. Good luck!</t>
   </si>
   <si>
-    <t>Quality of advice not sufficient, Time spent</t>
+    <t>Anxiety and/or panic attacks, Dry skin, Vaginal dryness, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t>Personalized recommendationson on how to address symptoms of menopause with the help of nutrition</t>
+  </si>
+  <si>
+    <t>I have no experience</t>
+  </si>
+  <si>
+    <t>traudel.sattler@gmail.com</t>
+  </si>
+  <si>
+    <t>guck luck for your reserch!</t>
+  </si>
+  <si>
+    <t>Money spent</t>
+  </si>
+  <si>
+    <t>Night sweats, Mood swings, Sleep difficulties, Low energy, fatigue, Dry mouth</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition, General recommendations on how to address menopause symptoms with the help of nutrition, Network of certified trusted nutritionists for online consultation, All of the above</t>
+  </si>
+  <si>
+    <t>Bloating, Hot flashes, Cold flashes, Headaches, Brain fog, Anxiety and/or panic attacks, Heart palpitations, Sleep difficulties, Joint pain, Low energy, fatigue, Dry skin, Dry mouth, Vaginal dryness</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition, Connection  with people who are at the same stage in their lives or have just been through it, General recommendations on how to address menopause symptoms with the help of nutrition, Network of certified trusted nutritionists for online consultation, One- click purchase of food supplements of trusted brands, All of the above</t>
+  </si>
+  <si>
+    <t>It saves time, It is private, I can do it as frequently as I want!</t>
+  </si>
+  <si>
+    <t>Night sweats, Body odor, Joint pain, Low energy, fatigue, Weight gain, Loss of skin elasticity, sagging skin, Skin wrinkling, Age spots, melasma, Dry skin, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t>I ask for advice when in the pharmacy</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition, Network of certified trusted nutritionists for online consultation, One- click purchase of food supplements of trusted brands</t>
+  </si>
+  <si>
+    <t>Maybe change the colours</t>
+  </si>
+  <si>
+    <t>s_puschiasis@yahoo.com</t>
+  </si>
+  <si>
+    <t>Gas, Night sweats, Hot flashes, Brain fog, Low energy, fatigue, Weight gain, Urinary tract infections, Loss of skin elasticity, sagging skin, Skin wrinkling, Age spots, melasma, Dry mouth, Vaginal dryness, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition, General recommendations on how to address menopause symptoms with the help of nutrition</t>
+  </si>
+  <si>
+    <t>familykropf@yahoo.com</t>
+  </si>
+  <si>
+    <t>You’re welcome</t>
+  </si>
+  <si>
+    <t>Constipation, Brain fog, Low energy, fatigue, Loss of skin elasticity, sagging skin, Vaginal dryness</t>
+  </si>
+  <si>
+    <t>General recommendations on how to address menopause symptoms with the help of nutrition</t>
+  </si>
+  <si>
+    <t>Anxiety and/or panic attacks, Loss of skin elasticity, sagging skin, Vaginal dryness, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m not informed yet. </t>
+  </si>
+  <si>
+    <t>Fraridu@yahoo.com</t>
+  </si>
+  <si>
+    <t>Thank you to you too !</t>
+  </si>
+  <si>
+    <t>Menstrual cramps, Depression, Joint pain, Weight gain, Loss of skin elasticity, sagging skin, Skin wrinkling, Age spots, melasma, Dry skin, Hair loss, thinning, change in texture</t>
+  </si>
+  <si>
+    <t>nadskia@hotmail.com</t>
+  </si>
+  <si>
+    <t>Money spent, Convenience of service</t>
+  </si>
+  <si>
+    <t>Constipation, Hot flashes, Body odor, Mood swings, Brain fog, Dry skin</t>
+  </si>
+  <si>
+    <t>I am aware of general healthy ways and try to stick to them, I follow advice from my doctors, I have always taken great care of my nutrition and health</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition</t>
+  </si>
+  <si>
+    <t>Maybe even in other languages</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Support myself in an ongoing transformation journey, Get myself out of a significant health issue, Prepare myself for the upcoming health challenge</t>
+  </si>
+  <si>
+    <t>Bloating, Gas, Body odor, Headaches, Sleep difficulties, Joint pain, Low energy, fatigue, Weight gain, Incontinence, Decreased memory</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition, General recommendations on how to address menopause symptoms with the help of nutrition, Network of certified trusted nutritionists for online consultation, One- click purchase of food supplements of trusted brands</t>
+  </si>
+  <si>
+    <t>gina.akadi@lazazzera.ch</t>
+  </si>
+  <si>
+    <t>Bloating, Sleep difficulties, Low energy, fatigue, Weight gain, Dry mouth</t>
+  </si>
+  <si>
+    <t>Personalized recommendations on how to address menopause symptoms with the help of nutrition, Network of certified trusted nutritionists for online consultation</t>
+  </si>
+  <si>
+    <t>emsiepitt@gmail.com</t>
+  </si>
+  <si>
+    <t>Night sweats, Mood swings, Heart palpitations, Low energy, fatigue, Weight gain</t>
+  </si>
+  <si>
+    <t>No app for health</t>
+  </si>
+  <si>
+    <t>Get myself out of a significant health issue, Prepare myself for the upcoming health challenge, Sortir du diabète</t>
+  </si>
+  <si>
+    <t>Gas, Heart palpitations, Weight gain, Bladder pain, frequent urination, Loss of skin elasticity, sagging skin, Decreased memory</t>
+  </si>
+  <si>
+    <t>Encore une app !!!!!!</t>
+  </si>
+  <si>
+    <t>La baisse des effets "ménopause-postménopause" est intéressante. Personnellement, je trouve chronophage et trop abstrait d'avoir à écouter le discours sur les bienfaits qui plus est en anglais. Je préfère une conférence sur le sujet avec la projection et les explications sur le rôle de l'app. Après ça, peut-être même volontaire pour essayer l'app...</t>
+  </si>
+  <si>
+    <t>voir plus haut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tout dépend de la fiabilité des "self-tests" </t>
+  </si>
+  <si>
+    <t>felanne.marie55@gmail.com</t>
+  </si>
+  <si>
+    <t>Mood swings, Loss of skin elasticity, sagging skin, Skin wrinkling, Age spots, melasma, Dry skin, Hair loss, thinning, change in texture</t>
   </si>
 </sst>
 </file>
@@ -3667,8 +4062,1834 @@
         <v>181</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="2">
+        <v>44670.70259006944</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="U29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD29" s="4">
+        <v>1982.0</v>
+      </c>
+      <c r="AE29" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF29" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG29" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH29" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AI29" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM29" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN29" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO29" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AR29" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2">
+        <v>44670.73628143518</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA30" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC30" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD30" s="4">
+        <v>1980.0</v>
+      </c>
+      <c r="AE30" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG30" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH30" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AI30" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM30" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN30" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2">
+        <v>44670.86206410879</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA31" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG31" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH31" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL31" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2">
+        <v>44671.3458021875</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA32" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB32" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD32" s="4">
+        <v>1975.0</v>
+      </c>
+      <c r="AE32" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG32" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH32" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AJ32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK32" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2">
+        <v>44676.91168621527</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="U33" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD33" s="4">
+        <v>1974.0</v>
+      </c>
+      <c r="AE33" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="AG33" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH33" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI33" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO33" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2">
+        <v>44680.31729445602</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="U34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z34" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD34" s="4">
+        <v>1973.0</v>
+      </c>
+      <c r="AG34" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH34" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AJ34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK34" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <v>44680.318009849536</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD35" s="4">
+        <v>1973.0</v>
+      </c>
+      <c r="AG35" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH35" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AJ35" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK35" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2">
+        <v>44680.32803837963</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA36" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD36" s="4">
+        <v>1973.0</v>
+      </c>
+      <c r="AG36" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH36" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AJ36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK36" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2">
+        <v>44685.29883569444</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z37" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA37" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC37" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD37" s="4">
+        <v>1976.0</v>
+      </c>
+      <c r="AE37" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG37" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH37" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI37" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO37" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2">
+        <v>44685.6425977662</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="U38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA38" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC38" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD38" s="4">
+        <v>1963.0</v>
+      </c>
+      <c r="AE38" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="AF38" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG38" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH38" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM38" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN38" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2">
+        <v>44685.71201177083</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="U39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z39" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA39" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC39" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD39" s="4">
+        <v>1986.0</v>
+      </c>
+      <c r="AE39" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="AG39" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH39" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI39" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM39" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN39" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO39" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AP39" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AQ39" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AR39" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AS39" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2">
+        <v>44685.93008186342</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="U40" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="V40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z40" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA40" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD40" s="4">
+        <v>1980.0</v>
+      </c>
+      <c r="AE40" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF40" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG40" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH40" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI40" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AJ40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN40" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO40" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2">
+        <v>44685.975979386574</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="U41" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z41" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC41" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD41" s="4">
+        <v>1970.0</v>
+      </c>
+      <c r="AE41" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AF41" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG41" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH41" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="AI41" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM41" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN41" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2">
+        <v>44686.16195275463</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="U42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="X42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z42" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA42" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD42" s="4">
+        <v>1980.0</v>
+      </c>
+      <c r="AE42" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG42" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH42" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AJ42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK42" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2">
+        <v>44686.31801371528</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="X43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA43" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD43" s="4">
+        <v>1977.0</v>
+      </c>
+      <c r="AE43" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF43" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="AG43" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH43" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AJ43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL43" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>44686.32109840278</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD44" s="4">
+        <v>1970.0</v>
+      </c>
+      <c r="AE44" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF44" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG44" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH44" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AI44" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR44" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>44686.5408818287</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="U45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA45" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB45" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC45" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD45" s="4">
+        <v>1980.0</v>
+      </c>
+      <c r="AE45" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="AF45" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG45" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH45" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AI45" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AJ45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM45" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN45" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO45" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AP45" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2">
+        <v>44686.60657905093</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="U46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB46" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC46" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD46" s="4">
+        <v>1955.0</v>
+      </c>
+      <c r="AE46" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF46" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AG46" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH46" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AJ46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN46" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2">
+        <v>44686.78336234954</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB47" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC47" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD47" s="4">
+        <v>1981.0</v>
+      </c>
+      <c r="AE47" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF47" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AG47" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH47" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="AI47" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO47" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2">
+        <v>44687.880361840274</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="X48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z48" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA48" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB48" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD48" s="4">
+        <v>1970.0</v>
+      </c>
+      <c r="AE48" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="AG48" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH48" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK48" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2">
+        <v>44690.69009082176</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="U49" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA49" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB49" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD49" s="4">
+        <v>1966.0</v>
+      </c>
+      <c r="AG49" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH49" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI49" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ49" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM49" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN49" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO49" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AP49" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2">
+        <v>44691.85146913194</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="U50" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z50" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA50" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB50" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC50" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>1981.0</v>
+      </c>
+      <c r="AG50" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH50" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO50" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2">
+        <v>44693.0820928125</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="U51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA51" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB51" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC51" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD51" s="4">
+        <v>1956.0</v>
+      </c>
+      <c r="AE51" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AF51" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="AG51" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="AH51" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI51" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AJ51" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN51" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO51" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3742,10 +5963,10 @@
         <v>33</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>205</v>
+        <v>293</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>206</v>
+        <v>294</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>36</v>
@@ -3754,73 +5975,73 @@
         <v>37</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>207</v>
+        <v>295</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>208</v>
+        <v>296</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>209</v>
+        <v>297</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>210</v>
+        <v>298</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>211</v>
+        <v>299</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>212</v>
+        <v>300</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>213</v>
+        <v>301</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>214</v>
+        <v>302</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>215</v>
+        <v>303</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>216</v>
+        <v>304</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>217</v>
+        <v>305</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>218</v>
+        <v>306</v>
       </c>
       <c r="AH1" s="4" t="s">
         <v>51</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>219</v>
+        <v>307</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>220</v>
+        <v>308</v>
       </c>
       <c r="AK1" s="4" t="s">
-        <v>221</v>
+        <v>309</v>
       </c>
       <c r="AL1" s="4" t="s">
-        <v>222</v>
+        <v>310</v>
       </c>
       <c r="AM1" s="4" t="s">
-        <v>223</v>
+        <v>311</v>
       </c>
       <c r="AN1" s="4" t="s">
-        <v>224</v>
+        <v>312</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>225</v>
+        <v>313</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>226</v>
+        <v>314</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>227</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2">
@@ -3831,7 +6052,7 @@
         <v>114</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>228</v>
+        <v>316</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>63</v>
@@ -3849,13 +6070,13 @@
         <v>67</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>229</v>
+        <v>317</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>77</v>
@@ -3870,7 +6091,7 @@
         <v>70</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>231</v>
+        <v>319</v>
       </c>
       <c r="AA2" s="4" t="s">
         <v>132</v>
@@ -3882,13 +6103,13 @@
         <v>160</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>232</v>
+        <v>320</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>233</v>
+        <v>321</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>234</v>
+        <v>322</v>
       </c>
       <c r="AG2" s="5"/>
       <c r="AH2" s="5"/>
@@ -3910,7 +6131,7 @@
         <v>87</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>235</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
@@ -3921,7 +6142,7 @@
         <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>236</v>
+        <v>324</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>64</v>
@@ -3948,7 +6169,7 @@
         <v>63</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>66</v>
@@ -3957,13 +6178,13 @@
         <v>67</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>238</v>
+        <v>326</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>239</v>
+        <v>327</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>118</v>
@@ -3978,7 +6199,7 @@
         <v>96</v>
       </c>
       <c r="Z4" s="4" t="s">
-        <v>240</v>
+        <v>328</v>
       </c>
       <c r="AA4" s="4" t="s">
         <v>159</v>
@@ -3987,10 +6208,10 @@
         <v>73</v>
       </c>
       <c r="AD4" s="8" t="s">
-        <v>241</v>
+        <v>329</v>
       </c>
       <c r="AE4" s="4" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5">
@@ -4001,7 +6222,7 @@
         <v>182</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>63</v>
@@ -4040,7 +6261,7 @@
         <v>105</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>73</v>
@@ -4052,10 +6273,10 @@
         <v>1974.0</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>245</v>
+        <v>333</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>246</v>
+        <v>334</v>
       </c>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
@@ -4077,7 +6298,7 @@
         <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>247</v>
+        <v>335</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>63</v>
@@ -4098,7 +6319,7 @@
         <v>87</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>15</v>
@@ -4139,7 +6360,7 @@
         <v>76</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>63</v>
@@ -4148,7 +6369,7 @@
         <v>63</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>250</v>
+        <v>336</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>86</v>
@@ -4198,13 +6419,13 @@
         <v>99</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>252</v>
+        <v>337</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>86</v>
@@ -4213,16 +6434,16 @@
         <v>87</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>253</v>
+        <v>338</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>254</v>
+        <v>339</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>255</v>
+        <v>340</v>
       </c>
       <c r="V8" s="4" t="s">
         <v>70</v>
@@ -4240,7 +6461,7 @@
         <v>89</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>256</v>
+        <v>341</v>
       </c>
       <c r="AB8" s="4" t="s">
         <v>111</v>
@@ -4252,7 +6473,7 @@
         <v>1957.0</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>257</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9">
@@ -4263,7 +6484,7 @@
         <v>83</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>258</v>
+        <v>343</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>63</v>
@@ -4299,10 +6520,10 @@
         <v>70</v>
       </c>
       <c r="Z9" s="4" t="s">
-        <v>259</v>
+        <v>344</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="AB9" s="4" t="s">
         <v>73</v>
@@ -4322,13 +6543,13 @@
         <v>99</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>261</v>
+        <v>345</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>63</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>262</v>
+        <v>346</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>102</v>
@@ -4337,13 +6558,13 @@
         <v>87</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>238</v>
+        <v>326</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>263</v>
+        <v>347</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>104</v>
@@ -4370,10 +6591,10 @@
         <v>1979.0</v>
       </c>
       <c r="AE10" s="4" t="s">
-        <v>264</v>
+        <v>348</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>265</v>
+        <v>349</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
@@ -4395,7 +6616,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>266</v>
+        <v>350</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>64</v>
@@ -4404,7 +6625,7 @@
         <v>64</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>102</v>
@@ -4413,7 +6634,7 @@
         <v>87</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>15</v>
@@ -4457,7 +6678,7 @@
         <v>83</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>269</v>
+        <v>352</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>63</v>
@@ -4475,10 +6696,10 @@
         <v>117</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>271</v>
+        <v>354</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>77</v>
@@ -4493,7 +6714,7 @@
         <v>70</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>272</v>
+        <v>355</v>
       </c>
       <c r="AA12" s="4" t="s">
         <v>106</v>
@@ -4508,10 +6729,10 @@
         <v>1979.0</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>273</v>
+        <v>356</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>274</v>
+        <v>357</v>
       </c>
       <c r="AG12" s="5"/>
       <c r="AH12" s="5"/>
@@ -4533,7 +6754,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>275</v>
+        <v>358</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>63</v>
@@ -4560,10 +6781,10 @@
         <v>121</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>276</v>
+        <v>359</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>77</v>
@@ -4584,7 +6805,7 @@
         <v>105</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>277</v>
+        <v>213</v>
       </c>
       <c r="AB13" s="4" t="s">
         <v>73</v>
@@ -4596,10 +6817,10 @@
         <v>1978.0</v>
       </c>
       <c r="AE13" s="4" t="s">
-        <v>278</v>
+        <v>360</v>
       </c>
       <c r="AF13" s="4" t="s">
-        <v>279</v>
+        <v>361</v>
       </c>
       <c r="AG13" s="5"/>
       <c r="AH13" s="5"/>
@@ -4621,7 +6842,7 @@
         <v>170</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>280</v>
+        <v>362</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>63</v>
@@ -4642,7 +6863,7 @@
         <v>67</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>281</v>
+        <v>363</v>
       </c>
       <c r="Q14" s="4" t="s">
         <v>15</v>
@@ -4675,7 +6896,7 @@
         <v>1969.0</v>
       </c>
       <c r="AE14" s="4" t="s">
-        <v>282</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15">
@@ -4683,10 +6904,10 @@
         <v>44654.80504972222</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>283</v>
+        <v>365</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>284</v>
+        <v>366</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>63</v>
@@ -4701,10 +6922,10 @@
         <v>143</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>285</v>
+        <v>367</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>285</v>
+        <v>367</v>
       </c>
       <c r="U15" s="4" t="s">
         <v>77</v>
@@ -4734,7 +6955,7 @@
         <v>1962.0</v>
       </c>
       <c r="AE15" s="4" t="s">
-        <v>286</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16">
@@ -4742,10 +6963,10 @@
         <v>44654.81236946759</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>287</v>
+        <v>369</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>288</v>
+        <v>370</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>64</v>
@@ -4760,7 +6981,7 @@
         <v>63</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>102</v>
@@ -4772,10 +6993,10 @@
         <v>103</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>290</v>
+        <v>372</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>77</v>
@@ -4805,10 +7026,10 @@
         <v>1979.0</v>
       </c>
       <c r="AE16" s="4" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="AF16" s="4" t="s">
-        <v>292</v>
+        <v>374</v>
       </c>
       <c r="AG16" s="5"/>
       <c r="AH16" s="5"/>
@@ -4830,13 +7051,13 @@
         <v>99</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>293</v>
+        <v>375</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>64</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>294</v>
+        <v>376</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>102</v>
@@ -4866,7 +7087,7 @@
         <v>89</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="AB17" s="4" t="s">
         <v>148</v>
@@ -4878,10 +7099,10 @@
         <v>1963.0</v>
       </c>
       <c r="AE17" s="4" t="s">
-        <v>295</v>
+        <v>377</v>
       </c>
       <c r="AF17" s="4" t="s">
-        <v>296</v>
+        <v>378</v>
       </c>
       <c r="AG17" s="5"/>
       <c r="AH17" s="5"/>
@@ -4903,7 +7124,7 @@
         <v>99</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>297</v>
+        <v>379</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>63</v>
@@ -4921,7 +7142,7 @@
         <v>143</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>298</v>
+        <v>380</v>
       </c>
       <c r="T18" s="4" t="s">
         <v>117</v>
@@ -4962,7 +7183,7 @@
         <v>99</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>299</v>
+        <v>381</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>64</v>
@@ -4977,7 +7198,7 @@
         <v>64</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>300</v>
+        <v>382</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>184</v>
@@ -4992,7 +7213,7 @@
         <v>15</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>301</v>
+        <v>383</v>
       </c>
       <c r="U19" s="4" t="s">
         <v>104</v>
@@ -5007,10 +7228,10 @@
         <v>70</v>
       </c>
       <c r="Z19" s="4" t="s">
-        <v>302</v>
+        <v>384</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="AB19" s="4" t="s">
         <v>111</v>
@@ -5022,10 +7243,10 @@
         <v>1965.0</v>
       </c>
       <c r="AE19" s="4" t="s">
-        <v>304</v>
+        <v>385</v>
       </c>
       <c r="AF19" s="4" t="s">
-        <v>305</v>
+        <v>386</v>
       </c>
       <c r="AG19" s="5"/>
       <c r="AH19" s="5"/>
@@ -5047,7 +7268,7 @@
         <v>76</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>306</v>
+        <v>387</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>63</v>
@@ -5098,7 +7319,7 @@
         <v>1975.0</v>
       </c>
       <c r="AE20" s="4" t="s">
-        <v>307</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21">
@@ -5109,7 +7330,7 @@
         <v>83</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>308</v>
+        <v>389</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>63</v>
@@ -5124,7 +7345,7 @@
         <v>63</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>102</v>
@@ -5171,7 +7392,7 @@
         <v>182</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>310</v>
+        <v>390</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>63</v>
@@ -5201,7 +7422,7 @@
         <v>15</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>311</v>
+        <v>391</v>
       </c>
       <c r="U22" s="4" t="s">
         <v>104</v>
@@ -5231,7 +7452,7 @@
         <v>1972.0</v>
       </c>
       <c r="AE22" s="4" t="s">
-        <v>312</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23">
@@ -5242,7 +7463,7 @@
         <v>99</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>313</v>
+        <v>393</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>63</v>
@@ -5299,10 +7520,10 @@
         <v>1963.0</v>
       </c>
       <c r="AE23" s="4" t="s">
-        <v>314</v>
+        <v>394</v>
       </c>
       <c r="AF23" s="4" t="s">
-        <v>234</v>
+        <v>322</v>
       </c>
       <c r="AG23" s="5"/>
       <c r="AH23" s="5"/>
@@ -5324,7 +7545,7 @@
         <v>182</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>315</v>
+        <v>395</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>63</v>
@@ -5363,7 +7584,7 @@
         <v>89</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>316</v>
+        <v>238</v>
       </c>
       <c r="AB24" s="4" t="s">
         <v>111</v>
@@ -5375,10 +7596,10 @@
         <v>1953.0</v>
       </c>
       <c r="AE24" s="4" t="s">
-        <v>317</v>
+        <v>396</v>
       </c>
       <c r="AG24" s="4" t="s">
-        <v>318</v>
+        <v>397</v>
       </c>
       <c r="AH24" s="5"/>
       <c r="AI24" s="5"/>
@@ -5399,7 +7620,7 @@
         <v>99</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>319</v>
+        <v>398</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>64</v>
@@ -5414,7 +7635,7 @@
         <v>64</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>320</v>
+        <v>399</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>66</v>
@@ -5426,10 +7647,10 @@
         <v>14</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>321</v>
+        <v>400</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>322</v>
+        <v>401</v>
       </c>
       <c r="U25" s="4" t="s">
         <v>104</v>
@@ -5462,7 +7683,7 @@
         <v>1982.0</v>
       </c>
       <c r="AE25" s="4" t="s">
-        <v>323</v>
+        <v>402</v>
       </c>
       <c r="AG25" s="4" t="s">
         <v>162</v>
@@ -5486,7 +7707,7 @@
         <v>99</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>324</v>
+        <v>403</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>63</v>
@@ -5513,10 +7734,10 @@
         <v>103</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>325</v>
+        <v>404</v>
       </c>
       <c r="U26" s="4" t="s">
         <v>104</v>
@@ -5549,7 +7770,7 @@
         <v>1971.0</v>
       </c>
       <c r="AG26" s="4" t="s">
-        <v>326</v>
+        <v>208</v>
       </c>
       <c r="AH26" s="5"/>
       <c r="AI26" s="5"/>
@@ -5570,7 +7791,7 @@
         <v>114</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>327</v>
+        <v>405</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>63</v>
@@ -5582,13 +7803,13 @@
         <v>63</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>328</v>
+        <v>406</v>
       </c>
       <c r="O27" s="4" t="s">
         <v>143</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>329</v>
+        <v>407</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>165</v>
@@ -5624,10 +7845,10 @@
         <v>1969.0</v>
       </c>
       <c r="AE27" s="4" t="s">
-        <v>330</v>
+        <v>408</v>
       </c>
       <c r="AF27" s="4" t="s">
-        <v>331</v>
+        <v>409</v>
       </c>
       <c r="AG27" s="4" t="s">
         <v>181</v>
@@ -5651,7 +7872,7 @@
         <v>83</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>63</v>
@@ -5663,13 +7884,13 @@
         <v>63</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>332</v>
+        <v>410</v>
       </c>
       <c r="O28" s="4" t="s">
         <v>143</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>333</v>
+        <v>411</v>
       </c>
       <c r="U28" s="4" t="s">
         <v>118</v>
@@ -5717,7 +7938,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>334</v>
+        <v>412</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>64</v>
@@ -5741,7 +7962,7 @@
         <v>15</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>335</v>
+        <v>413</v>
       </c>
       <c r="V29" s="4" t="s">
         <v>70</v>
@@ -5786,10 +8007,10 @@
         <v>44658.35834177083</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>336</v>
+        <v>414</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>337</v>
+        <v>415</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>63</v>
@@ -5798,7 +8019,7 @@
         <v>63</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>338</v>
+        <v>416</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>102</v>
@@ -5813,7 +8034,7 @@
         <v>15</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>339</v>
+        <v>417</v>
       </c>
       <c r="U30" s="4" t="s">
         <v>104</v>
@@ -5843,10 +8064,10 @@
         <v>1956.0</v>
       </c>
       <c r="AE30" s="4" t="s">
-        <v>340</v>
+        <v>418</v>
       </c>
       <c r="AF30" s="4" t="s">
-        <v>341</v>
+        <v>419</v>
       </c>
       <c r="AG30" s="4" t="s">
         <v>203</v>
@@ -5867,10 +8088,10 @@
         <v>44658.48133689815</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>342</v>
+        <v>420</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>343</v>
+        <v>421</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>136</v>
@@ -5879,10 +8100,10 @@
         <v>143</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>344</v>
+        <v>422</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>345</v>
+        <v>423</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>118</v>
@@ -5891,7 +8112,7 @@
         <v>70</v>
       </c>
       <c r="Z31" s="4" t="s">
-        <v>346</v>
+        <v>424</v>
       </c>
       <c r="AA31" s="4" t="s">
         <v>119</v>
@@ -5903,13 +8124,13 @@
         <v>1949.0</v>
       </c>
       <c r="AE31" s="4" t="s">
-        <v>347</v>
+        <v>425</v>
       </c>
       <c r="AF31" s="4" t="s">
-        <v>348</v>
+        <v>426</v>
       </c>
       <c r="AG31" s="4" t="s">
-        <v>349</v>
+        <v>427</v>
       </c>
       <c r="AH31" s="5"/>
       <c r="AI31" s="5"/>
@@ -5942,7 +8163,7 @@
         <v>143</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>333</v>
+        <v>411</v>
       </c>
       <c r="T32" s="4" t="s">
         <v>88</v>
@@ -5960,7 +8181,7 @@
         <v>1963.0</v>
       </c>
       <c r="AF32" s="4" t="s">
-        <v>350</v>
+        <v>428</v>
       </c>
       <c r="AG32" s="4" t="s">
         <v>181</v>
@@ -5984,7 +8205,7 @@
         <v>99</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>351</v>
+        <v>429</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>63</v>
@@ -6002,10 +8223,10 @@
         <v>87</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>352</v>
+        <v>430</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
       <c r="U33" s="4" t="s">
         <v>104</v>
@@ -6035,10 +8256,10 @@
         <v>1969.0</v>
       </c>
       <c r="AE33" s="4" t="s">
-        <v>353</v>
+        <v>431</v>
       </c>
       <c r="AF33" s="4" t="s">
-        <v>354</v>
+        <v>432</v>
       </c>
       <c r="AG33" s="4" t="s">
         <v>203</v>
@@ -6062,7 +8283,7 @@
         <v>182</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>355</v>
+        <v>433</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>64</v>
@@ -6113,10 +8334,10 @@
         <v>1964.0</v>
       </c>
       <c r="AE34" s="4" t="s">
-        <v>356</v>
+        <v>434</v>
       </c>
       <c r="AF34" s="4" t="s">
-        <v>357</v>
+        <v>435</v>
       </c>
       <c r="AG34" s="4" t="s">
         <v>203</v>
@@ -6140,7 +8361,7 @@
         <v>114</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>358</v>
+        <v>436</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>63</v>
@@ -6212,7 +8433,7 @@
         <v>76</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>359</v>
+        <v>437</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>63</v>
@@ -6227,7 +8448,7 @@
         <v>87</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>352</v>
+        <v>430</v>
       </c>
       <c r="Q36" s="4" t="s">
         <v>15</v>
@@ -6251,7 +8472,7 @@
         <v>105</v>
       </c>
       <c r="AA36" s="4" t="s">
-        <v>316</v>
+        <v>238</v>
       </c>
       <c r="AB36" s="4" t="s">
         <v>73</v>
@@ -6263,10 +8484,10 @@
         <v>1972.0</v>
       </c>
       <c r="AE36" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="AF36" s="4" t="s">
-        <v>361</v>
+        <v>439</v>
       </c>
       <c r="AG36" s="4" t="s">
         <v>203</v>
@@ -6283,13 +8504,13 @@
         <v>99</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>362</v>
+        <v>440</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>63</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>363</v>
+        <v>441</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>86</v>
@@ -6298,13 +8519,13 @@
         <v>143</v>
       </c>
       <c r="S37" s="4" t="s">
-        <v>333</v>
+        <v>411</v>
       </c>
       <c r="T37" s="4" t="s">
         <v>196</v>
       </c>
       <c r="U37" s="4" t="s">
-        <v>364</v>
+        <v>442</v>
       </c>
       <c r="V37" s="4" t="s">
         <v>70</v>
@@ -6345,10 +8566,10 @@
         <v>44664.50016859954</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>287</v>
+        <v>369</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>365</v>
+        <v>443</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>64</v>
@@ -6381,10 +8602,10 @@
         <v>14</v>
       </c>
       <c r="Q38" s="4" t="s">
-        <v>366</v>
+        <v>444</v>
       </c>
       <c r="R38" s="4" t="s">
-        <v>367</v>
+        <v>445</v>
       </c>
       <c r="U38" s="4" t="s">
         <v>104</v>
@@ -6405,7 +8626,7 @@
         <v>105</v>
       </c>
       <c r="AA38" s="4" t="s">
-        <v>368</v>
+        <v>446</v>
       </c>
       <c r="AB38" s="4" t="s">
         <v>73</v>
@@ -6417,25 +8638,25 @@
         <v>1972.0</v>
       </c>
       <c r="AE38" s="4" t="s">
-        <v>369</v>
+        <v>447</v>
       </c>
       <c r="AF38" s="4" t="s">
-        <v>370</v>
+        <v>448</v>
       </c>
       <c r="AG38" s="4" t="s">
-        <v>371</v>
+        <v>222</v>
       </c>
       <c r="AH38" s="4" t="s">
         <v>87</v>
       </c>
       <c r="AJ38" s="4" t="s">
-        <v>372</v>
+        <v>209</v>
       </c>
       <c r="AL38" s="4" t="s">
-        <v>373</v>
+        <v>449</v>
       </c>
       <c r="AM38" s="4" t="s">
-        <v>372</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39">
@@ -6446,7 +8667,7 @@
         <v>99</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>374</v>
+        <v>450</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>64</v>
@@ -6473,7 +8694,7 @@
         <v>15</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>375</v>
+        <v>451</v>
       </c>
       <c r="U39" s="4" t="s">
         <v>77</v>
@@ -6494,7 +8715,7 @@
         <v>105</v>
       </c>
       <c r="AA39" s="4" t="s">
-        <v>376</v>
+        <v>288</v>
       </c>
       <c r="AB39" s="4" t="s">
         <v>111</v>
@@ -6506,10 +8727,10 @@
         <v>1973.0</v>
       </c>
       <c r="AE39" s="4" t="s">
-        <v>377</v>
+        <v>452</v>
       </c>
       <c r="AF39" s="4" t="s">
-        <v>378</v>
+        <v>453</v>
       </c>
       <c r="AG39" s="4" t="s">
         <v>181</v>
@@ -6518,7 +8739,1108 @@
         <v>87</v>
       </c>
       <c r="AJ39" s="4" t="s">
-        <v>379</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2">
+        <v>44675.56264060186</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="S40" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="T40" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="U40" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="X40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z40" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA40" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD40" s="4">
+        <v>1954.0</v>
+      </c>
+      <c r="AE40" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="AF40" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="AG40" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ40" s="4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2">
+        <v>44675.950723483795</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2">
+        <v>44680.92522350694</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2">
+        <v>44684.79940416667</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z43" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="AA43" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC43" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD43" s="4">
+        <v>1969.0</v>
+      </c>
+      <c r="AG43" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ43" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AK43" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AQ43" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>44685.96977364583</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R44" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB44" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD44" s="4">
+        <v>1969.0</v>
+      </c>
+      <c r="AE44" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="AG44" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ44" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AK44" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AL44" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM44" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>44686.373830613426</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U45" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA45" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD45" s="4">
+        <v>1965.0</v>
+      </c>
+      <c r="AE45" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="AF45" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="AG45" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM45" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2">
+        <v>44686.461710069445</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB46" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC46" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD46" s="4">
+        <v>1965.0</v>
+      </c>
+      <c r="AG46" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH46" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2">
+        <v>44686.9100462037</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB47" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC47" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD47" s="4">
+        <v>1973.0</v>
+      </c>
+      <c r="AE47" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="AF47" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="AG47" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ47" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK47" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM47" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2">
+        <v>44686.9555934838</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z48" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA48" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB48" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC48" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD48" s="4">
+        <v>1978.0</v>
+      </c>
+      <c r="AE48" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="AG48" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ48" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="AL48" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM48" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2">
+        <v>44687.28445167824</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="R49" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="U49" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA49" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB49" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC49" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD49" s="4">
+        <v>1971.0</v>
+      </c>
+      <c r="AG49" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="AH49" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM49" s="4" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2">
+        <v>44687.46564625</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U50" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="V50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA50" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB50" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC50" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>1967.0</v>
+      </c>
+      <c r="AE50" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="AG50" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ50" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AK50" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AL50" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM50" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN50" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2">
+        <v>44687.765819594904</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U51" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z51" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA51" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC51" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD51" s="4">
+        <v>1966.0</v>
+      </c>
+      <c r="AE51" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="AF51" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG51" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH51" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ51" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AK51" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AL51" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>44687.82796782407</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="S52" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="T52" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="U52" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="X52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z52" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA52" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB52" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD52" s="4">
+        <v>1968.0</v>
+      </c>
+      <c r="AG52" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH52" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2">
+        <v>44691.50702239583</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P53" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q53" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="R53" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="U53" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="V53" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W53" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y53" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z53" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="AA53" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="AB53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC53" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD53" s="4">
+        <v>1955.0</v>
+      </c>
+      <c r="AE53" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="AG53" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH53" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ53" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>44692.903646516206</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="T54" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z54" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA54" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB54" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD54" s="4">
+        <v>1964.0</v>
+      </c>
+      <c r="AG54" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH54" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ54" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="AP54" s="4" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>